<commit_message>
Added the showing of soldes in user's profile and the fetch of soldes data from excel sheet
</commit_message>
<xml_diff>
--- a/oussama.xlsx
+++ b/oussama.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="1512" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GRH" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
   <si>
     <t>Code accès</t>
   </si>
@@ -178,6 +178,30 @@
   </si>
   <si>
     <t>Manager</t>
+  </si>
+  <si>
+    <t>Congé N</t>
+  </si>
+  <si>
+    <t>Congé N-1</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Site 01</t>
+  </si>
+  <si>
+    <t>Site 02</t>
+  </si>
+  <si>
+    <t>Site 03</t>
+  </si>
+  <si>
+    <t>Site 04</t>
+  </si>
+  <si>
+    <t>Site 05</t>
   </si>
 </sst>
 </file>
@@ -539,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -580,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,28 +616,37 @@
     <col min="2" max="2" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -623,18 +656,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -647,8 +681,17 @@
       <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -661,8 +704,17 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -675,8 +727,17 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -689,8 +750,17 @@
       <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -703,8 +773,17 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -717,8 +796,17 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -731,8 +819,17 @@
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -745,8 +842,17 @@
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -759,8 +865,17 @@
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -773,8 +888,17 @@
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -787,8 +911,17 @@
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -801,8 +934,17 @@
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -815,8 +957,17 @@
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -829,8 +980,17 @@
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -843,8 +1003,17 @@
       <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -857,8 +1026,17 @@
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -871,8 +1049,17 @@
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -885,8 +1072,17 @@
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
@@ -899,8 +1095,17 @@
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -913,8 +1118,17 @@
       <c r="D20" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -926,6 +1140,15 @@
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>